<commit_message>
+ Se verifica que el archivo a procesar exista
</commit_message>
<xml_diff>
--- a/mydata.xlsx
+++ b/mydata.xlsx
@@ -11,9 +11,10 @@
     <sheet name="Base" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Intermedia" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Punta" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Resumen Base" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Resumen Intermedia" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Resumen punta" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Resumen total" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Resumen Base" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Resumen Intermedia" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Resumen punta" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -20404,7 +20405,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20436,69 +20437,61 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="n">
-        <v>1998.453</v>
+        <v>11026.644</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Activa (KWh)</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>26.973</v>
-      </c>
-      <c r="C3" t="n">
-        <v>18.672</v>
-      </c>
-      <c r="D3" t="inlineStr"/>
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="n">
+        <v>1.599</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Fecha/hora</t>
-        </is>
-      </c>
-      <c r="B4" s="3" t="n">
-        <v>44565.09375</v>
-      </c>
-      <c r="C4" s="3" t="n">
-        <v>44566.21875</v>
+          <t>Activa (KWh)</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>71.33499999999999</v>
+      </c>
+      <c r="C4" t="n">
+        <v>13.223</v>
       </c>
       <c r="D4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Periodos</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>base</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>base</t>
-        </is>
+          <t>Fecha/hora</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>44565.77083333334</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>44568.35416666666</v>
       </c>
       <c r="D5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>TR1.</t>
+          <t>Periodos</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>02:15:00</t>
+          <t>punta</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>05:15:00</t>
+          <t>intermedia</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
@@ -20506,30 +20499,48 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>TR1.E.Reactiva</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0</v>
+          <t>TR1.</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>18:30:00</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>08:30:00</t>
+        </is>
       </c>
       <c r="D7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
+          <t>TR1.E.Reactiva</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
           <t>tarifas</t>
         </is>
       </c>
-      <c r="B8" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" t="inlineStr"/>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -20542,7 +20553,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20574,69 +20585,61 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="n">
-        <v>7014.857</v>
+        <v>1998.453</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Activa (KWh)</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>68.41800000000001</v>
-      </c>
-      <c r="C3" t="n">
-        <v>13.223</v>
-      </c>
-      <c r="D3" t="inlineStr"/>
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Fecha/hora</t>
-        </is>
-      </c>
-      <c r="B4" s="3" t="n">
-        <v>44565.73958333334</v>
-      </c>
-      <c r="C4" s="3" t="n">
-        <v>44568.35416666666</v>
+          <t>Activa (KWh)</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>26.973</v>
+      </c>
+      <c r="C4" t="n">
+        <v>18.672</v>
       </c>
       <c r="D4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Periodos</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>intermedia</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>intermedia</t>
-        </is>
+          <t>Fecha/hora</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>44565.09375</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>44566.21875</v>
       </c>
       <c r="D5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>TR1.</t>
+          <t>Periodos</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>17:45:00</t>
+          <t>base</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>08:30:00</t>
+          <t>base</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
@@ -20644,30 +20647,48 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>TR1.E.Reactiva</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0</v>
+          <t>TR1.</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>02:15:00</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>05:15:00</t>
+        </is>
       </c>
       <c r="D7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
+          <t>TR1.E.Reactiva</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
           <t>tarifas</t>
         </is>
       </c>
-      <c r="B8" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" t="inlineStr"/>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -20680,7 +20701,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20712,69 +20733,61 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="n">
-        <v>2013.334</v>
+        <v>7014.857</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Activa (KWh)</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>71.33499999999999</v>
-      </c>
-      <c r="C3" t="n">
-        <v>19.603</v>
-      </c>
-      <c r="D3" t="inlineStr"/>
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="n">
+        <v>1.599</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Fecha/hora</t>
-        </is>
-      </c>
-      <c r="B4" s="3" t="n">
-        <v>44565.77083333334</v>
-      </c>
-      <c r="C4" s="3" t="n">
-        <v>44565.89583333334</v>
+          <t>Activa (KWh)</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>68.41800000000001</v>
+      </c>
+      <c r="C4" t="n">
+        <v>13.223</v>
       </c>
       <c r="D4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Periodos</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>punta</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>punta</t>
-        </is>
+          <t>Fecha/hora</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>44565.73958333334</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>44568.35416666666</v>
       </c>
       <c r="D5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>TR1.</t>
+          <t>Periodos</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>18:30:00</t>
+          <t>intermedia</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>21:30:00</t>
+          <t>intermedia</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
@@ -20782,30 +20795,196 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>TR1.E.Reactiva</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0</v>
+          <t>TR1.</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>17:45:00</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>08:30:00</t>
+        </is>
       </c>
       <c r="D7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
+          <t>TR1.E.Reactiva</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
           <t>tarifas</t>
         </is>
       </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Demanda Maxima</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Demanda Minima</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>consumo total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="n">
+        <v>2013.334</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Activa (KWh)</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>71.33499999999999</v>
+      </c>
+      <c r="C4" t="n">
+        <v>19.603</v>
+      </c>
+      <c r="D4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Fecha/hora</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>44565.77083333334</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>44565.89583333334</v>
+      </c>
+      <c r="D5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Periodos</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>punta</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>punta</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>TR1.</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>18:30:00</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>21:30:00</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>TR1.E.Reactiva</t>
+        </is>
+      </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>tarifas</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>